<commit_message>
Update Website & Meilensteintrendanalyse
</commit_message>
<xml_diff>
--- a/Plan/Meilensteintrendanalyse.xlsx
+++ b/Plan/Meilensteintrendanalyse.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stefa\OneDrive\Desktop\SYP-Projekt\Plan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8E5763D-71C1-4AAC-9281-9DD90EE6FDD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACB95F17-540E-47A9-87F3-0365D036BC7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{14DC5C8D-CF8B-47DD-B602-BCCBE3CB0C77}"/>
   </bookViews>
@@ -439,6 +439,10 @@
     <xf numFmtId="14" fontId="0" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -469,10 +473,6 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -784,6 +784,9 @@
                 <c:pt idx="1">
                   <c:v>45072</c:v>
                 </c:pt>
+                <c:pt idx="2">
+                  <c:v>45009</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -911,6 +914,9 @@
                   <c:v>45023</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>45023</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>45023</c:v>
                 </c:pt>
               </c:numCache>
@@ -1450,6 +1456,9 @@
                   <c:v>45079</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>45079</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>45079</c:v>
                 </c:pt>
               </c:numCache>
@@ -3043,7 +3052,7 @@
   <dimension ref="A1:ER569"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="O34" sqref="O34"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3058,39 +3067,39 @@
   <sheetData>
     <row r="1" spans="2:148" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:148" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B2" s="27" t="s">
+      <c r="B2" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="28"/>
-      <c r="D2" s="29" t="s">
+      <c r="C2" s="32"/>
+      <c r="D2" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
       <c r="G2" s="4"/>
     </row>
     <row r="3" spans="2:148" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B3" s="34" t="s">
+      <c r="B3" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="35"/>
-      <c r="D3" s="30" t="s">
+      <c r="C3" s="39"/>
+      <c r="D3" s="34" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="30"/>
-      <c r="F3" s="30"/>
+      <c r="E3" s="34"/>
+      <c r="F3" s="34"/>
       <c r="G3" s="4"/>
     </row>
     <row r="4" spans="2:148" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B4" s="31" t="s">
+      <c r="B4" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="32"/>
-      <c r="D4" s="33">
+      <c r="C4" s="36"/>
+      <c r="D4" s="37">
         <v>44986</v>
       </c>
-      <c r="E4" s="30"/>
-      <c r="F4" s="30"/>
+      <c r="E4" s="34"/>
+      <c r="F4" s="34"/>
       <c r="G4" s="4"/>
     </row>
     <row r="5" spans="2:148" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3103,25 +3112,25 @@
       <c r="B7" s="6"/>
       <c r="C7" s="7"/>
       <c r="D7" s="7"/>
-      <c r="E7" s="26" t="s">
+      <c r="E7" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="F7" s="26"/>
-      <c r="G7" s="26"/>
-      <c r="H7" s="26"/>
-      <c r="I7" s="26"/>
-      <c r="J7" s="26"/>
-      <c r="K7" s="26"/>
-      <c r="L7" s="26"/>
-      <c r="M7" s="26"/>
-      <c r="N7" s="26"/>
-      <c r="O7" s="26"/>
-      <c r="P7" s="26"/>
-      <c r="Q7" s="26"/>
-      <c r="R7" s="26"/>
-      <c r="S7" s="26"/>
-      <c r="T7" s="26"/>
-      <c r="U7" s="26"/>
+      <c r="F7" s="30"/>
+      <c r="G7" s="30"/>
+      <c r="H7" s="30"/>
+      <c r="I7" s="30"/>
+      <c r="J7" s="30"/>
+      <c r="K7" s="30"/>
+      <c r="L7" s="30"/>
+      <c r="M7" s="30"/>
+      <c r="N7" s="30"/>
+      <c r="O7" s="30"/>
+      <c r="P7" s="30"/>
+      <c r="Q7" s="30"/>
+      <c r="R7" s="30"/>
+      <c r="S7" s="30"/>
+      <c r="T7" s="30"/>
+      <c r="U7" s="30"/>
     </row>
     <row r="8" spans="2:148" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="16" t="s">
@@ -3323,23 +3332,23 @@
       <c r="F9" s="19">
         <v>45016</v>
       </c>
-      <c r="G9" s="36">
+      <c r="G9" s="26">
         <v>44988</v>
       </c>
-      <c r="H9" s="36"/>
-      <c r="I9" s="36"/>
-      <c r="J9" s="36"/>
-      <c r="K9" s="36"/>
-      <c r="L9" s="36"/>
-      <c r="M9" s="36"/>
-      <c r="N9" s="36"/>
-      <c r="O9" s="36"/>
-      <c r="P9" s="36"/>
-      <c r="Q9" s="36"/>
-      <c r="R9" s="36"/>
-      <c r="S9" s="36"/>
-      <c r="T9" s="36"/>
-      <c r="U9" s="39"/>
+      <c r="H9" s="26"/>
+      <c r="I9" s="26"/>
+      <c r="J9" s="26"/>
+      <c r="K9" s="26"/>
+      <c r="L9" s="26"/>
+      <c r="M9" s="26"/>
+      <c r="N9" s="26"/>
+      <c r="O9" s="26"/>
+      <c r="P9" s="26"/>
+      <c r="Q9" s="26"/>
+      <c r="R9" s="26"/>
+      <c r="S9" s="26"/>
+      <c r="T9" s="26"/>
+      <c r="U9" s="29"/>
       <c r="AA9" s="1"/>
       <c r="AB9" s="1"/>
       <c r="AC9" s="1"/>
@@ -3479,7 +3488,9 @@
       <c r="F10" s="11">
         <v>45072</v>
       </c>
-      <c r="G10" s="12"/>
+      <c r="G10" s="12">
+        <v>45009</v>
+      </c>
       <c r="H10" s="12"/>
       <c r="I10" s="12"/>
       <c r="J10" s="12"/>
@@ -3633,7 +3644,9 @@
       <c r="F11" s="11">
         <v>45023</v>
       </c>
-      <c r="G11" s="12"/>
+      <c r="G11" s="12">
+        <v>45023</v>
+      </c>
       <c r="H11" s="12"/>
       <c r="I11" s="12"/>
       <c r="J11" s="12"/>
@@ -3787,23 +3800,23 @@
       <c r="F12" s="11">
         <v>45065</v>
       </c>
-      <c r="G12" s="36">
+      <c r="G12" s="26">
         <v>44988</v>
       </c>
-      <c r="H12" s="36"/>
-      <c r="I12" s="36"/>
-      <c r="J12" s="36"/>
-      <c r="K12" s="36"/>
-      <c r="L12" s="36"/>
-      <c r="M12" s="36"/>
-      <c r="N12" s="36"/>
-      <c r="O12" s="36"/>
-      <c r="P12" s="36"/>
-      <c r="Q12" s="36"/>
-      <c r="R12" s="36"/>
-      <c r="S12" s="36"/>
-      <c r="T12" s="36"/>
-      <c r="U12" s="37"/>
+      <c r="H12" s="26"/>
+      <c r="I12" s="26"/>
+      <c r="J12" s="26"/>
+      <c r="K12" s="26"/>
+      <c r="L12" s="26"/>
+      <c r="M12" s="26"/>
+      <c r="N12" s="26"/>
+      <c r="O12" s="26"/>
+      <c r="P12" s="26"/>
+      <c r="Q12" s="26"/>
+      <c r="R12" s="26"/>
+      <c r="S12" s="26"/>
+      <c r="T12" s="26"/>
+      <c r="U12" s="27"/>
       <c r="AA12" s="1"/>
       <c r="AB12" s="1"/>
       <c r="AC12" s="1"/>
@@ -4255,7 +4268,9 @@
       <c r="F15" s="11">
         <v>45079</v>
       </c>
-      <c r="G15" s="12"/>
+      <c r="G15" s="12">
+        <v>45079</v>
+      </c>
       <c r="H15" s="12"/>
       <c r="I15" s="12"/>
       <c r="J15" s="12"/>
@@ -4451,7 +4466,7 @@
       <c r="T16" s="21">
         <v>45086</v>
       </c>
-      <c r="U16" s="38">
+      <c r="U16" s="28">
         <v>45086</v>
       </c>
       <c r="AA16" s="1"/>

</xml_diff>